<commit_message>
add the comparison of CitySim.
minor fix and rename column archive
</commit_message>
<xml_diff>
--- a/xlsx_ouputs/cooling_with_citysim.xlsx
+++ b/xlsx_ouputs/cooling_with_citysim.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
-    <t>ESP</t>
-  </si>
-  <si>
-    <t>BLAST</t>
-  </si>
-  <si>
-    <t>DOE2</t>
-  </si>
-  <si>
-    <t>SRES/SUN</t>
-  </si>
-  <si>
-    <t>SERIRES</t>
-  </si>
-  <si>
-    <t>S3PAS</t>
-  </si>
-  <si>
-    <t>TRNSYS</t>
-  </si>
-  <si>
-    <t>TASE</t>
+    <t>ESP(AC)</t>
+  </si>
+  <si>
+    <t>BLAST(AC)</t>
+  </si>
+  <si>
+    <t>DOE2(AC)</t>
+  </si>
+  <si>
+    <t>SRES/SUN(AC)</t>
+  </si>
+  <si>
+    <t>SERIRES(AC)</t>
+  </si>
+  <si>
+    <t>S3PAS(AC)</t>
+  </si>
+  <si>
+    <t>TRNSYS(AC)</t>
+  </si>
+  <si>
+    <t>TASE(AC)</t>
   </si>
   <si>
     <t>min</t>
@@ -998,7 +998,7 @@
         <v>0.51</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1267,7 +1267,7 @@
         <v>1.86</v>
       </c>
       <c r="M18">
-        <v>-15</v>
+        <v>-14.6</v>
       </c>
     </row>
     <row r="19" spans="1:13">

</xml_diff>